<commit_message>
actualizando excel de aforo
</commit_message>
<xml_diff>
--- a/uploads/MATRIZ_PLATAFORMA_MASTER.xlsx
+++ b/uploads/MATRIZ_PLATAFORMA_MASTER.xlsx
@@ -7035,7 +7035,7 @@
         <v>INICIAL</v>
       </c>
       <c r="C10">
-        <v>INGRESAR EL AFORO POR CADA AMBIENTE SELECCIONADO</v>
+        <v>NaN</v>
       </c>
       <c r="D10">
         <f>SUM(D11:D17)</f>
@@ -7078,7 +7078,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D11">
         <f>B11*C11</f>
@@ -7129,7 +7129,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <f>B12*C12</f>
@@ -7180,7 +7180,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D13">
         <f>B13*C13</f>
@@ -7447,7 +7447,7 @@
         <v>1.3</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D20">
         <f>B20*C20</f>
@@ -7492,7 +7492,7 @@
         <v>1.3</v>
       </c>
       <c r="C21">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D21">
         <f>B21*C21</f>
@@ -7537,7 +7537,7 @@
         <v>1.3</v>
       </c>
       <c r="C22">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D22">
         <f>B22*C22</f>
@@ -7582,7 +7582,7 @@
         <v>1.3</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D23">
         <f>B23*C23</f>
@@ -7627,7 +7627,7 @@
         <v>1.3</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D24">
         <f>B24*C24</f>
@@ -7672,7 +7672,7 @@
         <v>1.3</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="D25">
         <f>B25*C25</f>
@@ -7794,7 +7794,7 @@
         <v>1.4</v>
       </c>
       <c r="C29">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D29">
         <f>B29*C29</f>
@@ -7826,7 +7826,7 @@
         <v>1.4</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D30">
         <f>B30*C30</f>
@@ -7858,7 +7858,7 @@
         <v>1.4</v>
       </c>
       <c r="C31">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D31">
         <f>B31*C31</f>
@@ -7890,7 +7890,7 @@
         <v>1.4</v>
       </c>
       <c r="C32">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D32">
         <f>B32*C32</f>
@@ -7922,7 +7922,7 @@
         <v>1.4</v>
       </c>
       <c r="C33">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D33">
         <f>B33*C33</f>

</xml_diff>

<commit_message>
fixes for mysql server
</commit_message>
<xml_diff>
--- a/uploads/MATRIZ_PLATAFORMA_MASTER.xlsx
+++ b/uploads/MATRIZ_PLATAFORMA_MASTER.xlsx
@@ -7035,7 +7035,7 @@
         <v>INICIAL</v>
       </c>
       <c r="C10">
-        <v>INGRESAR EL AFORO POR CADA AMBIENTE SELECCIONADO</v>
+        <v>NaN</v>
       </c>
       <c r="D10">
         <f>SUM(D11:D17)</f>
@@ -7078,7 +7078,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <f>B11*C11</f>
@@ -7129,7 +7129,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <f>B12*C12</f>
@@ -7180,7 +7180,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <f>B13*C13</f>
@@ -7447,7 +7447,7 @@
         <v>1.3</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D20">
         <f>B20*C20</f>
@@ -7492,7 +7492,7 @@
         <v>1.3</v>
       </c>
       <c r="C21">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D21">
         <f>B21*C21</f>
@@ -7537,7 +7537,7 @@
         <v>1.3</v>
       </c>
       <c r="C22">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D22">
         <f>B22*C22</f>
@@ -7582,7 +7582,7 @@
         <v>1.3</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D23">
         <f>B23*C23</f>
@@ -7627,7 +7627,7 @@
         <v>1.3</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D24">
         <f>B24*C24</f>
@@ -7672,7 +7672,7 @@
         <v>1.3</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="D25">
         <f>B25*C25</f>
@@ -7794,7 +7794,7 @@
         <v>1.4</v>
       </c>
       <c r="C29">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D29">
         <f>B29*C29</f>
@@ -7826,7 +7826,7 @@
         <v>1.4</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D30">
         <f>B30*C30</f>
@@ -7858,7 +7858,7 @@
         <v>1.4</v>
       </c>
       <c r="C31">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D31">
         <f>B31*C31</f>
@@ -7890,7 +7890,7 @@
         <v>1.4</v>
       </c>
       <c r="C32">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D32">
         <f>B32*C32</f>
@@ -7922,7 +7922,7 @@
         <v>1.4</v>
       </c>
       <c r="C33">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D33">
         <f>B33*C33</f>

</xml_diff>